<commit_message>
Added node functioanlity to search
</commit_message>
<xml_diff>
--- a/backend/ExportedInventory.xlsx
+++ b/backend/ExportedInventory.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" windowHeight="9660" windowWidth="16095" xWindow="240" yWindow="15"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,25 +78,188 @@
   <si>
     <t>Nintendo</t>
   </si>
+  <si>
+    <t xml:space="preserve">Wii Sports	nan	Wii.jfif	82	40	Nintendo
+Super Mario Bros.	nan	NES.jfif	40	20	Nintendo
+Mario Kart Wii	nan	Wii.jfif	35	40	Nintendo
+Wii Sports Resort	nan	Wii.jfif	33	40	Nintendo
+Pokemon Red/Pokemon Blue	nan	GB.jfif	31	20	Nintendo
+Tetris	nan	GB.jfif	30	20	Nintendo
+New Super Mario Bros.	nan	DS.jfif	30	40	Nintendo
+Wii Play	nan	Wii.jfif	29	40	Nintendo
+New Super Mario Bros. Wii	nan	Wii.jfif	28	40	Nintendo
+Duck Hunt	nan	NES.jfif	28	20	Nintendo
+Nintendogs	nan	DS.jfif	24	40	Nintendo
+Mario Kart DS	nan	DS.jfif	23	40	Nintendo
+Pokemon Gold/Pokemon Silver	nan	GB.jfif	23	20	Nintendo
+Wii Fit	nan	Wii.jfif	22	40	Nintendo
+Wii Fit Plus	nan	Wii.jfif	22	40	Nintendo
+Kinect Adventures!	nan	X360.jfif	21	40	Microsoft Game Studios
+Grand Theft Auto V	nan	PS3.jfif	21	50	Take-Two Interactive
+Grand Theft Auto: San Andreas	nan	PS2.jfif	20	40	Take-Two Interactive
+Super Mario World	nan	SNES.jfif	20	20	Nintendo
+Brain Age: Train Your Brain in Minutes a Day	nan	DS.jfif	20	40	Nintendo
+Pokemon Diamond/Pokemon Pearl	nan	DS.jfif	18	40	Nintendo
+Super Mario Land	nan	GB.jfif	18	20	Nintendo
+Super Mario Bros. 3	nan	NES.jfif	17	20	Nintendo
+Grand Theft Auto V	nan	X360.jfif	16	50	Take-Two Interactive
+Grand Theft Auto: Vice City	nan	PS2.jfif	16	40	Take-Two Interactive
+Pokemon Ruby/Pokemon Sapphire	nan	GBA.jfif	15	40	Nintendo
+Pokemon Black/Pokemon White	nan	DS.jfif	15	40	Nintendo
+Brain Age 2: More Training in Minutes a Day	nan	DS.jfif	15	40	Nintendo
+Gran Turismo 3: A-Spec	nan	PS2.jfif	14	40	Sony Computer Entertainment
+Call of Duty: Modern Warfare 3	nan	X360.jfif	14	50	Activision
+Pokémon Yellow: Special Pikachu Edition	nan	GB.jfif	14	20	Nintendo
+Call of Duty: Black Ops	nan	X360.jfif	14	40	Activision
+Pokemon X/Pokemon Y	nan	3DS.jfif	14	50	Nintendo
+Call of Duty: Black Ops 3	nan	PS4.jfif	14	50	Activision
+Call of Duty: Black Ops II	nan	PS3.jfif	14	50	Activision
+Call of Duty: Black Ops II	nan	X360.jfif	13	50	Activision
+Call of Duty: Modern Warfare 2	nan	X360.jfif	13	40	Activision
+Call of Duty: Modern Warfare 3	nan	PS3.jfif	13	50	Activision
+Grand Theft Auto III	nan	PS2.jfif	13	40	Take-Two Interactive
+Super Smash Bros. Brawl	nan	Wii.jfif	13	40	Nintendo
+Call of Duty: Black Ops	nan	PS3.jfif	12	40	Activision
+Animal Crossing: Wild World	nan	DS.jfif	12	40	Nintendo
+Mario Kart 7	nan	3DS.jfif	12	50	Nintendo
+Halo 3	nan	X360.jfif	12	40	Microsoft Game Studios
+Grand Theft Auto V	nan	PS4.jfif	11	50	Take-Two Interactive
+Pokemon HeartGold/Pokemon SoulSilver	nan	DS.jfif	11	40	Nintendo
+Super Mario 64	nan	N64.jfif	11	20	Nintendo
+Gran Turismo 4	nan	PS2.jfif	11	40	Sony Computer Entertainment
+Super Mario Galaxy	nan	Wii.jfif	11	40	Nintendo
+Pokemon Omega Ruby/Pokemon Alpha Sapphire	nan	3DS.jfif	11	50	Nintendo
+Super Mario Land 2: 6 Golden Coins	nan	GB.jfif	11	20	Nintendo
+Grand Theft Auto IV	nan	X360.jfif	11	40	Take-Two Interactive
+Gran Turismo	nan	PS.jfif	10	20	Sony Computer Entertainment
+Super Mario 3D Land	nan	3DS.jfif	10	50	Nintendo
+Gran Turismo 5	nan	PS3.jfif	10	40	Sony Computer Entertainment
+Call of Duty: Modern Warfare 2	nan	PS3.jfif	10	40	Activision
+Grand Theft Auto IV	nan	PS3.jfif	10	40	Take-Two Interactive
+Super Mario All-Stars	nan	SNES.jfif	10	20	Nintendo
+Pokemon FireRed/Pokemon LeafGreen	nan	GBA.jfif	10	40	Nintendo
+Super Mario 64	nan	DS.jfif	10	40	Nintendo
+Just Dance 3	nan	Wii.jfif	10	50	Ubisoft
+Call of Duty: Ghosts	nan	X360.jfif	10	50	Activision
+Halo: Reach	nan	X360.jfif	9	40	Microsoft Game Studios
+Mario Kart 64	nan	N64.jfif	9	20	Nintendo
+New Super Mario Bros. 2	nan	3DS.jfif	9	50	Nintendo
+Halo 4	nan	X360.jfif	9	50	Microsoft Game Studios
+Final Fantasy VII	nan	PS.jfif	9	20	Sony Computer Entertainment
+Call of Duty: Ghosts	nan	PS3.jfif	9	50	Activision
+Just Dance 2	nan	Wii.jfif	9	40	Ubisoft
+Gran Turismo 2	nan	PS.jfif	9	20	Sony Computer Entertainment
+Call of Duty 4: Modern Warfare	nan	X360.jfif	9	40	Activision
+Donkey Kong Country	nan	SNES.jfif	9	20	Nintendo
+Minecraft	nan	X360.jfif	9	50	Microsoft Game Studios
+Animal Crossing: New Leaf	nan	3DS.jfif	9	50	Nintendo
+Mario Party DS	nan	DS.jfif	9	40	Nintendo
+The Elder Scrolls V: Skyrim	nan	X360.jfif	8	50	Bethesda Softworks
+Super Mario Kart	nan	SNES.jfif	8	20	Nintendo
+FIFA 16	nan	PS4.jfif	8	50	Electronic Arts
+Wii Party	nan	Wii.jfif	8	40	Nintendo
+Halo 2	nan	XB.jfif	8	40	Microsoft Game Studios
+Mario Party 8	nan	Wii.jfif	8	40	Nintendo
+Pokemon Black 2/Pokemon White 2	nan	DS.jfif	8	50	Nintendo
+FIFA Soccer 13	nan	PS3.jfif	8	50	Electronic Arts
+The Sims 3	nan	PC.jfif	8	40	Electronic Arts
+GoldenEye 007	nan	N64.jfif	8	20	Nintendo
+Mario &amp; Sonic at the Olympic Games	nan	Wii.jfif	8	40	Sega
+Final Fantasy X	nan	PS2.jfif	8	40	Sony Computer Entertainment
+Final Fantasy VIII	nan	PS.jfif	7	20	SquareSoft
+Pokémon Platinum Version	nan	DS.jfif	7	40	Nintendo
+Grand Theft Auto: Liberty City Stories	nan	PSP.jfif	7	40	Take-Two Interactive
+Super Mario Galaxy 2	nan	Wii.jfif	7	40	Nintendo
+Star Wars Battlefront (2015)	nan	PS4.jfif	7	50	Electronic Arts
+Call of Duty: Advanced Warfare	nan	PS4.jfif	7	50	Activision
+The Legend of Zelda: Ocarina of Time	nan	N64.jfif	7	20	Nintendo
+Crash Bandicoot 2: Cortex Strikes Back	nan	PS.jfif	7	20	Sony Computer Entertainment
+Super Mario Bros. 2	nan	NES.jfif	7	20	Nintendo
+Super Smash Bros. for Wii U and 3DS	nan	3DS.jfif	7	50	Nintendo
+Call of Duty: World at War	nan	X360.jfif	7	40	Activision
+Battlefield 3	nan	X360.jfif	7	50	Electronic Arts
+The Legend of Zelda: Twilight Princess	nan	Wii.jfif	7	40	Nintendo
+Call of Duty: Black Ops 3	nan	XOne.jfif	7	50	Activision
+Just Dance	nan	Wii.jfif	7	40	Ubisoft
+Battlefield 3	nan	PS3.jfif	7	50	Electronic Arts
+Need for Speed Underground	nan	PS2.jfif	7	40	Electronic Arts
+Tekken 3	nan	PS.jfif	7	20	Sony Computer Entertainment
+Crash Bandicoot 3: Warped	nan	PS.jfif	7	20	Sony Computer Entertainment
+Super Smash Bros. Melee	nan	GC.jfif	7	40	Nintendo
+Mario Kart 8	nan	WiiU.jfif	6	50	Nintendo
+Fallout 4	nan	PS4.jfif	6	50	Bethesda Softworks
+Mario Kart: Double Dash!!	nan	GC.jfif	6	40	Nintendo
+Just Dance 4	nan	Wii.jfif	6	50	Ubisoft
+FIFA 14	nan	PS3.jfif	6	50	Electronic Arts
+Need for Speed Underground 2	nan	PS2.jfif	6	40	Electronic Arts
+Medal of Honor: Frontline	nan	PS2.jfif	6	40	Electronic Arts
+Uncharted 3: Drake's Deception	nan	PS3.jfif	6	50	Sony Computer Entertainment
+Crash Bandicoot	nan	PS.jfif	6	20	Sony Computer Entertainment
+Zumba Fitness	nan	Wii.jfif	6	40	505 Games
+Gears of War 2	nan	X360.jfif	6	40	Microsoft Game Studios
+Uncharted 2: Among Thieves	nan	PS3.jfif	6	40	Sony Computer Entertainment
+Call of Duty 4: Modern Warfare	nan	PS3.jfif	6	40	Activision
+FIFA 12	nan	PS3.jfif	6	50	Electronic Arts
+Big Brain Academy	nan	DS.jfif	6	40	Nintendo
+Red Dead Redemption	nan	PS3.jfif	6	40	Take-Two Interactive
+FIFA 15	nan	PS4.jfif	6	50	Electronic Arts
+Donkey Kong Country Returns	nan	Wii.jfif	6	40	Nintendo
+The Elder Scrolls V: Skyrim	nan	PS3.jfif	6	50	Bethesda Softworks
+The Legend of Zelda	nan	NES.jfif	6	20	Nintendo
+Assassin's Creed III	nan	PS3.jfif	6	50	Ubisoft
+Halo: Combat Evolved	nan	XB.jfif	6	40	Microsoft Game Studios
+Pokémon Emerald Version	nan	GBA.jfif	6	40	Nintendo
+Kingdom Hearts	nan	PS2.jfif	6	40	Sony Computer Entertainment
+Pokémon Crystal Version	nan	GB.jfif	6	20	Nintendo
+Halo 3: ODST	nan	X360.jfif	6	40	Microsoft Game Studios
+Red Dead Redemption	nan	X360.jfif	6	40	Take-Two Interactive
+Super Mario Sunshine	nan	GC.jfif	6	40	Nintendo
+Street Fighter II: The World Warrior	nan	SNES.jfif	6	20	Capcom
+World of Warcraft	nan	PC.jfif	6	40	Activision
+Driver	nan	PS.jfif	6	20	GT Interactive
+Kinect Sports	nan	X360.jfif	6	40	Microsoft Game Studios
+Gears of War 3	nan	X360.jfif	6	50	Microsoft Game Studios
+Gears of War	nan	X360.jfif	6	40	Microsoft Game Studios
+Metal Gear Solid 2: Sons of Liberty	nan	PS2.jfif	6	40	Konami Digital Entertainment
+Metal Gear Solid 4: Guns of the Patriots	nan	PS3.jfif	6	40	Konami Digital Entertainment
+Metal Gear Solid	nan	PS.jfif	6	20	Konami Digital Entertainment
+The Last of Us	nan	PS3.jfif	5	50	Sony Computer Entertainment Europe
+Final Fantasy XII	nan	PS2.jfif	5	40	Square Enix
+LittleBigPlanet	nan	PS3.jfif	5	40	Sony Computer Entertainment
+Dragon Quest IX: Sentinels of the Starry Skies	nan	DS.jfif	5	40	Nintendo
+LEGO Star Wars: The Complete Saga	nan	Wii.jfif	5	40	LucasArts
+Resident Evil 2	nan	PS.jfif	5	20	Virgin Interactive
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -110,30 +273,42 @@
   </fills>
   <borders count="2">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -433,12 +608,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection pane="topLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">

</xml_diff>